<commit_message>
lots of progress, now the program has a nice and working web-page like graphical interface
</commit_message>
<xml_diff>
--- a/App/Data/data_base.xlsx
+++ b/App/Data/data_base.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="25">
   <si>
     <t xml:space="preserve">Nombre</t>
   </si>
@@ -28,12 +28,18 @@
     <t xml:space="preserve">Numero</t>
   </si>
   <si>
+    <t xml:space="preserve">Categoria</t>
+  </si>
+  <si>
     <t xml:space="preserve">Hora de salida</t>
   </si>
   <si>
     <t xml:space="preserve">Juana</t>
   </si>
   <si>
+    <t xml:space="preserve">Perros</t>
+  </si>
+  <si>
     <t xml:space="preserve">Carlitos</t>
   </si>
   <si>
@@ -49,6 +55,9 @@
     <t xml:space="preserve">Pancha</t>
   </si>
   <si>
+    <t xml:space="preserve">Gatos</t>
+  </si>
+  <si>
     <t xml:space="preserve">Carlota</t>
   </si>
   <si>
@@ -68,6 +77,9 @@
   </si>
   <si>
     <t xml:space="preserve">Bob esponja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chivos</t>
   </si>
   <si>
     <t xml:space="preserve">El hombre araña</t>
@@ -194,15 +206,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
+      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.63"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -215,203 +229,260 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="C2" s="2" t="n">
-        <v>0.353472222222222</v>
+        <v>14</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>0.0208333333333333</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>143</v>
       </c>
-      <c r="C3" s="2" t="n">
-        <v>0.353472222222222</v>
+      <c r="C3" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>0.0208333333333333</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>53</v>
       </c>
-      <c r="C4" s="2" t="n">
-        <v>0.353472222222222</v>
+      <c r="C4" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>0.0208333333333334</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>141</v>
       </c>
-      <c r="C5" s="2" t="n">
-        <v>0.353472222222222</v>
+      <c r="C5" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>0.0208333333333334</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>98</v>
       </c>
-      <c r="C6" s="2" t="n">
-        <v>0.353472222222222</v>
+      <c r="C6" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>0.0208333333333334</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>231</v>
       </c>
-      <c r="C7" s="2" t="n">
-        <v>0.353472222222222</v>
+      <c r="C7" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>0.0208333333333335</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>214</v>
       </c>
-      <c r="C8" s="2" t="n">
-        <v>0.353472222222222</v>
+      <c r="C8" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>0.0208333333333335</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>52</v>
       </c>
-      <c r="C9" s="2" t="n">
-        <v>0.353472222222222</v>
+      <c r="C9" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="2" t="n">
+        <v>0.0208333333333335</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="C10" s="2" t="n">
-        <v>0.353472222222222</v>
+      <c r="C10" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>0.0208333333333336</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>64</v>
       </c>
-      <c r="C11" s="2" t="n">
-        <v>0.353472222222222</v>
+      <c r="C11" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="2" t="n">
+        <v>0.0208333333333336</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>241</v>
       </c>
-      <c r="C12" s="2" t="n">
-        <v>0.353472222222222</v>
+      <c r="C12" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="2" t="n">
+        <v>0.0208333333333336</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>86</v>
       </c>
-      <c r="C13" s="2" t="n">
-        <v>0.353472222222222</v>
+      <c r="C13" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="2" t="n">
+        <v>0.0208333333333336</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>45</v>
       </c>
-      <c r="C14" s="2" t="n">
-        <v>0.353472222222222</v>
+      <c r="C14" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="2" t="n">
+        <v>0.0208333333333337</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>36</v>
       </c>
-      <c r="C15" s="2" t="n">
-        <v>0.353472222222222</v>
+      <c r="C15" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="2" t="n">
+        <v>0.0208333333333337</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>32</v>
       </c>
-      <c r="C16" s="2" t="n">
-        <v>0.353472222222222</v>
+      <c r="C16" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="2" t="n">
+        <v>0.0208333333333337</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>76</v>
       </c>
-      <c r="C17" s="2" t="n">
-        <v>0.353472222222222</v>
+      <c r="C17" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="2" t="n">
+        <v>0.0208333333333338</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>23</v>
       </c>
-      <c r="C18" s="2" t="n">
-        <v>0.353472222222222</v>
+      <c r="C18" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="2" t="n">
+        <v>0.0208333333333338</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>67</v>
       </c>
-      <c r="C19" s="2" t="n">
-        <v>0.353472222222222</v>
+      <c r="C19" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="2" t="n">
+        <v>0.0208333333333338</v>
       </c>
     </row>
   </sheetData>

</xml_diff>